<commit_message>
Added 34Hz Filter Manual Bode Plot
</commit_message>
<xml_diff>
--- a/Dades en Llaç obert.xlsx
+++ b/Dades en Llaç obert.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{882FFD21-1B27-40D7-B1F7-00E6313C494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46544317-8FCA-400F-A9E0-6C970E017122}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dades en Llaç obert" sheetId="1" r:id="rId1"/>
+    <sheet name="Mot, Tac, Pot, ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="Passabaixos 34Hz" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Angle</t>
   </si>
@@ -116,12 +116,33 @@
   </si>
   <si>
     <t>Angle 2 rad</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vin </t>
+  </si>
+  <si>
+    <t>Pk-Pk</t>
+  </si>
+  <si>
+    <t>Mitjà</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Delay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,6 +562,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9359E7-2D80-4013-93A0-C952FEBF81FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V28" sqref="V28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,4 +2422,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="42"/>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="42">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="42"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="42"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="42"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="42">
+        <v>1</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="42">
+        <v>10</v>
+      </c>
+      <c r="C8" s="42">
+        <v>6.65</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="42">
+        <v>6.3</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="42">
+        <v>-17</v>
+      </c>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
+        <v>20</v>
+      </c>
+      <c r="C9" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D9" s="42">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="42">
+        <v>5.7</v>
+      </c>
+      <c r="F9" s="42">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="G9" s="42">
+        <v>-30</v>
+      </c>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="42">
+        <v>30</v>
+      </c>
+      <c r="C10" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E10" s="42">
+        <v>5</v>
+      </c>
+      <c r="F10" s="42">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="G10" s="42">
+        <v>-40</v>
+      </c>
+      <c r="H10" s="42"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="42">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="C11" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D11" s="42">
+        <v>-0.25</v>
+      </c>
+      <c r="E11" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="F11" s="42">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="G11" s="42">
+        <v>-45</v>
+      </c>
+      <c r="H11" s="42"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="42">
+        <v>50</v>
+      </c>
+      <c r="C12" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D12" s="42">
+        <v>-0.02</v>
+      </c>
+      <c r="E12" s="42">
+        <v>3.84</v>
+      </c>
+      <c r="F12" s="42">
+        <v>-0.03</v>
+      </c>
+      <c r="G12" s="42">
+        <v>-52</v>
+      </c>
+      <c r="H12" s="42"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="42">
+        <v>100</v>
+      </c>
+      <c r="C13" s="42">
+        <v>6.64</v>
+      </c>
+      <c r="D13" s="42">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="E13" s="42">
+        <v>2.36</v>
+      </c>
+      <c r="F13" s="42">
+        <v>-0.03</v>
+      </c>
+      <c r="G13" s="42">
+        <v>-67</v>
+      </c>
+      <c r="H13" s="42"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="42">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D14" s="42">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F14" s="42">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="G14" s="42">
+        <v>-80</v>
+      </c>
+      <c r="H14" s="42"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="42">
+        <v>10000</v>
+      </c>
+      <c r="C15" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="D15" s="42">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="42">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="42"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+    </row>
+    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Derivative action bode plot | Added Filter Bode datapoints | Added bode plots data processing live script
</commit_message>
<xml_diff>
--- a/Dades en Llaç obert.xlsx
+++ b/Dades en Llaç obert.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03F8D5-BB67-4235-AEBA-4FF4B584A22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mot, Tac, Pot, ADC" sheetId="1" r:id="rId1"/>
-    <sheet name="Passabaixos 34Hz" sheetId="2" r:id="rId2"/>
+    <sheet name="Motor  Tac. Pot. i ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="Bodes Filtre i Derivador" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Angle</t>
   </si>
@@ -138,12 +139,30 @@
   <si>
     <t>Delay</t>
   </si>
+  <si>
+    <t>Filtre 34Hz</t>
+  </si>
+  <si>
+    <t>Derivador</t>
+  </si>
+  <si>
+    <t>Guany 0,1</t>
+  </si>
+  <si>
+    <t>Guany 0,01</t>
+  </si>
+  <si>
+    <t>Saturació</t>
+  </si>
+  <si>
+    <t>Anomalies</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +223,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -249,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -446,11 +479,511 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,11 +1099,192 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,11 +1599,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,340 +3139,661 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="91"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="68"/>
+    </row>
+    <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="104" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="84"/>
+      <c r="M3" s="87"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43" t="s">
+      <c r="D4" s="82"/>
+      <c r="E4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="44"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="F4" s="80"/>
+      <c r="G4" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="63"/>
+      <c r="J4" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="58"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D5" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G5" s="65"/>
+      <c r="H5" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="89"/>
+      <c r="K5" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="65"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="47">
+        <v>1</v>
+      </c>
+      <c r="C6" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D6" s="60">
+        <v>0.08</v>
+      </c>
+      <c r="E6" s="55">
+        <v>6.5</v>
+      </c>
+      <c r="F6" s="53">
+        <v>0.02</v>
+      </c>
+      <c r="G6" s="43">
+        <f>-360*8.8/1000</f>
+        <v>-3.1680000000000006</v>
+      </c>
+      <c r="H6" s="55">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I6" s="53">
+        <v>-0.1</v>
+      </c>
+      <c r="J6" s="95">
+        <v>97</v>
+      </c>
+      <c r="K6" s="55">
+        <v>0.65</v>
+      </c>
+      <c r="L6" s="53">
+        <v>-0.01</v>
+      </c>
+      <c r="M6" s="43">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="47">
+        <v>2</v>
+      </c>
+      <c r="C7" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D7" s="60">
+        <v>-0.05</v>
+      </c>
+      <c r="E7" s="55">
+        <v>6.5</v>
+      </c>
+      <c r="F7" s="53">
+        <v>-0.05</v>
+      </c>
+      <c r="G7" s="43">
+        <f>-360*2*4.4/1000</f>
+        <v>-3.1680000000000006</v>
+      </c>
+      <c r="H7" s="55">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I7" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>88</v>
+      </c>
+      <c r="K7" s="55">
+        <v>1</v>
+      </c>
+      <c r="L7" s="53">
+        <v>-0.01</v>
+      </c>
+      <c r="M7" s="43">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="47">
+        <v>3</v>
+      </c>
+      <c r="C8" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D8" s="60">
+        <v>-0.63</v>
+      </c>
+      <c r="E8" s="55">
+        <v>6.5</v>
+      </c>
+      <c r="F8" s="53">
+        <v>-0.06</v>
+      </c>
+      <c r="G8" s="43">
+        <v>-5.5</v>
+      </c>
+      <c r="H8" s="55">
+        <v>12.4</v>
+      </c>
+      <c r="I8" s="57">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>87</v>
+      </c>
+      <c r="K8" s="55">
+        <v>1.44</v>
+      </c>
+      <c r="L8" s="53">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="M8" s="43">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="47">
+        <v>5</v>
+      </c>
+      <c r="C9" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0.27</v>
+      </c>
+      <c r="E9" s="55">
+        <v>6.45</v>
+      </c>
+      <c r="F9" s="53">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G9" s="43">
+        <v>-9</v>
+      </c>
+      <c r="H9" s="55">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I9" s="53">
+        <v>0.4</v>
+      </c>
+      <c r="J9" s="4">
+        <v>87</v>
+      </c>
+      <c r="K9" s="55">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L9" s="53">
+        <v>-0.01</v>
+      </c>
+      <c r="M9" s="43">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="47">
+        <v>10</v>
+      </c>
+      <c r="C10" s="51">
+        <v>6.65</v>
+      </c>
+      <c r="D10" s="60">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="55">
+        <v>6.3</v>
+      </c>
+      <c r="F10" s="53">
+        <v>0.02</v>
+      </c>
+      <c r="G10" s="43">
+        <v>-17</v>
+      </c>
+      <c r="H10" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I10" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>74</v>
+      </c>
+      <c r="K10" s="55">
+        <v>4.2</v>
+      </c>
+      <c r="L10" s="53">
+        <v>-0.02</v>
+      </c>
+      <c r="M10" s="43">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="47">
+        <v>15</v>
+      </c>
+      <c r="C11" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D11" s="60">
+        <v>-0.06</v>
+      </c>
+      <c r="E11" s="55">
+        <v>6</v>
+      </c>
+      <c r="F11" s="53">
+        <v>-0.01</v>
+      </c>
+      <c r="G11" s="43">
+        <v>-23.5</v>
+      </c>
+      <c r="H11" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I11" s="53">
+        <v>0.13</v>
+      </c>
+      <c r="J11" s="4">
+        <v>60</v>
+      </c>
+      <c r="K11" s="55">
+        <v>6.2</v>
+      </c>
+      <c r="L11" s="53">
+        <v>-0.02</v>
+      </c>
+      <c r="M11" s="43">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="47">
+        <v>20</v>
+      </c>
+      <c r="C12" s="51">
+        <v>6.6</v>
+      </c>
+      <c r="D12" s="60">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="E12" s="55">
+        <v>5.7</v>
+      </c>
+      <c r="F12" s="53">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="G12" s="43">
+        <v>-30</v>
+      </c>
+      <c r="H12" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I12" s="53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J12" s="4">
+        <v>53</v>
+      </c>
+      <c r="K12" s="55">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L12" s="53">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M12" s="43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="47">
+        <v>30</v>
+      </c>
+      <c r="C13" s="51">
+        <v>6.6</v>
+      </c>
+      <c r="D13" s="60">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E13" s="55">
+        <v>5</v>
+      </c>
+      <c r="F13" s="53">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="G13" s="43">
+        <v>-40</v>
+      </c>
+      <c r="H13" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I13" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="J13" s="4">
+        <v>44</v>
+      </c>
+      <c r="K13" s="55">
+        <v>12.2</v>
+      </c>
+      <c r="L13" s="53">
+        <v>0.01</v>
+      </c>
+      <c r="M13" s="43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="47">
+        <v>34</v>
+      </c>
+      <c r="C14" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D14" s="60">
+        <v>-0.01</v>
+      </c>
+      <c r="E14" s="55">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F14" s="53">
+        <v>-0.04</v>
+      </c>
+      <c r="G14" s="43">
+        <v>-43</v>
+      </c>
+      <c r="H14" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I14" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>41</v>
+      </c>
+      <c r="K14" s="55">
+        <v>13.6</v>
+      </c>
+      <c r="L14" s="53">
+        <v>-0.06</v>
+      </c>
+      <c r="M14" s="43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="47">
+        <v>40</v>
+      </c>
+      <c r="C15" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="D15" s="60">
+        <v>-0.02</v>
+      </c>
+      <c r="E15" s="55">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F15" s="53">
+        <v>-0.05</v>
+      </c>
+      <c r="G15" s="43">
+        <v>-46</v>
+      </c>
+      <c r="H15" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I15" s="53">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>38</v>
+      </c>
+      <c r="K15" s="55">
+        <v>16.2</v>
+      </c>
+      <c r="L15" s="53">
+        <v>2E-3</v>
+      </c>
+      <c r="M15" s="43">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="47">
+        <v>50</v>
+      </c>
+      <c r="C16" s="51">
+        <v>6.6</v>
+      </c>
+      <c r="D16" s="60">
+        <v>-0.02</v>
+      </c>
+      <c r="E16" s="55">
+        <v>3.84</v>
+      </c>
+      <c r="F16" s="53">
+        <v>-0.03</v>
+      </c>
+      <c r="G16" s="43">
+        <v>-52</v>
+      </c>
+      <c r="H16" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I16" s="53">
+        <v>0.04</v>
+      </c>
+      <c r="J16" s="4">
         <v>33</v>
       </c>
-      <c r="H3" s="42"/>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="42">
-        <v>1E-3</v>
-      </c>
-      <c r="C4" s="42" t="s">
+      <c r="K16" s="55">
+        <v>20</v>
+      </c>
+      <c r="L16" s="53">
+        <v>0</v>
+      </c>
+      <c r="M16" s="43">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="47">
+        <v>100</v>
+      </c>
+      <c r="C17" s="51">
+        <v>6.64</v>
+      </c>
+      <c r="D17" s="60">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="E17" s="55">
+        <v>2.36</v>
+      </c>
+      <c r="F17" s="53">
+        <v>-0.03</v>
+      </c>
+      <c r="G17" s="43">
+        <v>-67</v>
+      </c>
+      <c r="H17" s="92">
+        <v>21.2</v>
+      </c>
+      <c r="I17" s="53">
+        <v>0.03</v>
+      </c>
+      <c r="J17" s="4">
+        <v>18</v>
+      </c>
+      <c r="K17" s="90">
+        <v>21.2</v>
+      </c>
+      <c r="L17" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="M17" s="43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="47">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="51">
+        <v>6.6</v>
+      </c>
+      <c r="D18" s="60">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E18" s="55">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F18" s="53">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="G18" s="43">
+        <v>-80</v>
+      </c>
+      <c r="H18" s="93">
+        <v>0</v>
+      </c>
+      <c r="I18" s="94">
+        <v>0</v>
+      </c>
+      <c r="J18" s="95">
+        <v>0</v>
+      </c>
+      <c r="K18" s="93">
+        <v>0</v>
+      </c>
+      <c r="L18" s="94">
+        <v>0</v>
+      </c>
+      <c r="M18" s="96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="48">
+        <v>10000</v>
+      </c>
+      <c r="C19" s="52">
+        <v>6.6</v>
+      </c>
+      <c r="D19" s="61">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E19" s="56">
+        <v>0.05</v>
+      </c>
+      <c r="F19" s="54">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="G19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="42"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="42">
-        <v>0.01</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="42"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="42">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="42"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="42">
-        <v>1</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="42"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="42">
-        <v>10</v>
-      </c>
-      <c r="C8" s="42">
-        <v>6.65</v>
-      </c>
-      <c r="D8" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="E8" s="42">
-        <v>6.3</v>
-      </c>
-      <c r="F8" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="G8" s="42">
-        <v>-17</v>
-      </c>
-      <c r="H8" s="42"/>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="42">
-        <v>20</v>
-      </c>
-      <c r="C9" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D9" s="42">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="E9" s="42">
-        <v>5.7</v>
-      </c>
-      <c r="F9" s="42">
-        <v>-2.5999999999999999E-2</v>
-      </c>
-      <c r="G9" s="42">
-        <v>-30</v>
-      </c>
-      <c r="H9" s="42"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="42">
-        <v>30</v>
-      </c>
-      <c r="C10" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D10" s="42">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E10" s="42">
-        <v>5</v>
-      </c>
-      <c r="F10" s="42">
-        <v>-3.3000000000000002E-2</v>
-      </c>
-      <c r="G10" s="42">
-        <v>-40</v>
-      </c>
-      <c r="H10" s="42"/>
-    </row>
-    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="42">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="C11" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D11" s="42">
-        <v>-0.25</v>
-      </c>
-      <c r="E11" s="42">
-        <v>4.7</v>
-      </c>
-      <c r="F11" s="42">
-        <v>-6.0000000000000001E-3</v>
-      </c>
-      <c r="G11" s="42">
-        <v>-45</v>
-      </c>
-      <c r="H11" s="42"/>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="42">
-        <v>50</v>
-      </c>
-      <c r="C12" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D12" s="42">
-        <v>-0.02</v>
-      </c>
-      <c r="E12" s="42">
-        <v>3.84</v>
-      </c>
-      <c r="F12" s="42">
-        <v>-0.03</v>
-      </c>
-      <c r="G12" s="42">
-        <v>-52</v>
-      </c>
-      <c r="H12" s="42"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="42">
-        <v>100</v>
-      </c>
-      <c r="C13" s="42">
-        <v>6.64</v>
-      </c>
-      <c r="D13" s="42">
-        <v>-1.4999999999999999E-2</v>
-      </c>
-      <c r="E13" s="42">
-        <v>2.36</v>
-      </c>
-      <c r="F13" s="42">
-        <v>-0.03</v>
-      </c>
-      <c r="G13" s="42">
-        <v>-67</v>
-      </c>
-      <c r="H13" s="42"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="42">
-        <v>1000</v>
-      </c>
-      <c r="C14" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D14" s="42">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E14" s="42">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F14" s="42">
-        <v>-3.4000000000000002E-2</v>
-      </c>
-      <c r="G14" s="42">
-        <v>-80</v>
-      </c>
-      <c r="H14" s="42"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="42">
-        <v>10000</v>
-      </c>
-      <c r="C15" s="42">
-        <v>6.6</v>
-      </c>
-      <c r="D15" s="42">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="E15" s="42">
-        <v>0.05</v>
-      </c>
-      <c r="F15" s="42">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="G15" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="42"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="97">
+        <v>8.6</v>
+      </c>
+      <c r="I19" s="98">
+        <v>5.3</v>
+      </c>
+      <c r="J19" s="99">
+        <v>-120</v>
+      </c>
+      <c r="K19" s="97">
+        <v>8.6</v>
+      </c>
+      <c r="L19" s="98">
+        <v>5.3</v>
+      </c>
+      <c r="M19" s="100">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-    </row>
-    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>
@@ -2767,34 +3802,35 @@
       <c r="G22" s="42"/>
       <c r="H22" s="42"/>
     </row>
-    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23" s="101"/>
+      <c r="I23" s="101"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
       <c r="C24" s="42"/>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+    </row>
+    <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
@@ -2803,7 +3839,7 @@
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
     </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="42"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
@@ -2812,7 +3848,7 @@
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
     </row>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="42"/>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
@@ -2821,7 +3857,7 @@
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
     </row>
-    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>
@@ -2830,16 +3866,15 @@
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
     </row>
-    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
       <c r="D30" s="42"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
       <c r="H30" s="42"/>
     </row>
-    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
@@ -2848,7 +3883,7 @@
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
     </row>
-    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
@@ -2858,9 +3893,21 @@
       <c r="H32" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
+  <mergeCells count="14">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="J4:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
First approach to PWM control
</commit_message>
<xml_diff>
--- a/Dades en Llaç obert.xlsx
+++ b/Dades en Llaç obert.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03F8D5-BB67-4235-AEBA-4FF4B584A22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motor  Tac. Pot. i ADC" sheetId="1" r:id="rId1"/>
-    <sheet name="Bodes Filtre i Derivador" sheetId="2" r:id="rId2"/>
+    <sheet name="PWM en llaç obert" sheetId="3" r:id="rId2"/>
+    <sheet name="Bodes Filtre i Derivador" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Angle</t>
   </si>
@@ -156,12 +156,27 @@
   </si>
   <si>
     <t>Anomalies</t>
+  </si>
+  <si>
+    <t>% DC</t>
+  </si>
+  <si>
+    <t>Ton</t>
+  </si>
+  <si>
+    <t>Freqüència</t>
+  </si>
+  <si>
+    <t>Amplada</t>
+  </si>
+  <si>
+    <t>Escala Ton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1154,94 +1169,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1277,6 +1205,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1284,6 +1215,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1599,11 +1614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="B3" sqref="B3:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,10 +3154,479 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="42">
+        <v>-5</v>
+      </c>
+      <c r="C4" s="42">
+        <f>ABS(B4)/$C$34*100</f>
+        <v>100</v>
+      </c>
+      <c r="D4" s="42">
+        <f>1/$C$33*(C4)/100*$C$35</f>
+        <v>500</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="42">
+        <v>-4.5</v>
+      </c>
+      <c r="C5" s="42">
+        <f t="shared" ref="C5:C30" si="0">ABS(B5)/$C$34*100</f>
+        <v>90</v>
+      </c>
+      <c r="D5" s="42">
+        <f t="shared" ref="D5:D30" si="1">1/$C$33*(C5)/100*$C$35</f>
+        <v>450</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="42">
+        <v>-4</v>
+      </c>
+      <c r="C6" s="42">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D6" s="42">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="42">
+        <v>-3.5</v>
+      </c>
+      <c r="C7" s="42">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D7" s="42">
+        <f t="shared" si="1"/>
+        <v>350.00000000000006</v>
+      </c>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="42">
+        <v>-3</v>
+      </c>
+      <c r="C8" s="42">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D8" s="42">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
+        <v>-2.5</v>
+      </c>
+      <c r="C9" s="42">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D9" s="42">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="42">
+        <v>-2</v>
+      </c>
+      <c r="C10" s="42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D10" s="42">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="42">
+        <v>-1.5</v>
+      </c>
+      <c r="C11" s="42">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D11" s="42">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="42">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="42">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D12" s="42">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="42">
+        <v>-0.8</v>
+      </c>
+      <c r="C13" s="42">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="42">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="42">
+        <v>-0.6</v>
+      </c>
+      <c r="C14" s="42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D14" s="42">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="42">
+        <v>-0.4</v>
+      </c>
+      <c r="C15" s="42">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="42">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="42">
+        <v>-0.2</v>
+      </c>
+      <c r="C16" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D16" s="42">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="42">
+        <v>0</v>
+      </c>
+      <c r="C17" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D18" s="42">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="C19" s="42">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D19" s="42">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="C20" s="42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D20" s="42">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="42">
+        <v>0.8</v>
+      </c>
+      <c r="C21" s="42">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="42">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="42">
+        <v>1</v>
+      </c>
+      <c r="C22" s="42">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="42">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="C23" s="42">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D23" s="42">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="42">
+        <v>2</v>
+      </c>
+      <c r="C24" s="42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D24" s="42">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="C25" s="42">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D25" s="42">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="42">
+        <v>3</v>
+      </c>
+      <c r="C26" s="42">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D26" s="42">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="42">
+        <v>3.5</v>
+      </c>
+      <c r="C27" s="42">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D27" s="42">
+        <f t="shared" si="1"/>
+        <v>350.00000000000006</v>
+      </c>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="42">
+        <v>4</v>
+      </c>
+      <c r="C28" s="42">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D28" s="42">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="42">
+        <v>4.5</v>
+      </c>
+      <c r="C29" s="42">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D29" s="42">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="42">
+        <v>5</v>
+      </c>
+      <c r="C30" s="42">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D30" s="42">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -3150,79 +3634,79 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="69" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="66" t="s">
+      <c r="F2" s="86"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="68"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="83" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86" t="s">
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="84"/>
-      <c r="M3" s="87"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="103"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="79" t="s">
+      <c r="D4" s="98"/>
+      <c r="E4" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="78" t="s">
+      <c r="F4" s="96"/>
+      <c r="G4" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="88" t="s">
+      <c r="I4" s="79"/>
+      <c r="J4" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="63"/>
-      <c r="M4" s="64" t="s">
+      <c r="L4" s="79"/>
+      <c r="M4" s="80" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
-      <c r="B5" s="76"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="44" t="s">
         <v>29</v>
       </c>
@@ -3235,21 +3719,21 @@
       <c r="F5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="65"/>
+      <c r="G5" s="81"/>
       <c r="H5" s="45" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="89"/>
+      <c r="J5" s="105"/>
       <c r="K5" s="45" t="s">
         <v>29</v>
       </c>
       <c r="L5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="65"/>
+      <c r="M5" s="81"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="47">
@@ -3277,7 +3761,7 @@
       <c r="I6" s="53">
         <v>-0.1</v>
       </c>
-      <c r="J6" s="95">
+      <c r="J6" s="66">
         <v>97</v>
       </c>
       <c r="K6" s="55">
@@ -3424,7 +3908,7 @@
       <c r="G10" s="43">
         <v>-17</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="63">
         <v>21.2</v>
       </c>
       <c r="I10" s="53">
@@ -3462,7 +3946,7 @@
       <c r="G11" s="43">
         <v>-23.5</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="63">
         <v>21.2</v>
       </c>
       <c r="I11" s="53">
@@ -3500,7 +3984,7 @@
       <c r="G12" s="43">
         <v>-30</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="63">
         <v>21.2</v>
       </c>
       <c r="I12" s="53">
@@ -3538,7 +4022,7 @@
       <c r="G13" s="43">
         <v>-40</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="63">
         <v>21.2</v>
       </c>
       <c r="I13" s="53">
@@ -3576,7 +4060,7 @@
       <c r="G14" s="43">
         <v>-43</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="63">
         <v>21.2</v>
       </c>
       <c r="I14" s="53">
@@ -3614,7 +4098,7 @@
       <c r="G15" s="43">
         <v>-46</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="63">
         <v>21.2</v>
       </c>
       <c r="I15" s="53">
@@ -3652,7 +4136,7 @@
       <c r="G16" s="43">
         <v>-52</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="63">
         <v>21.2</v>
       </c>
       <c r="I16" s="53">
@@ -3690,7 +4174,7 @@
       <c r="G17" s="43">
         <v>-67</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="63">
         <v>21.2</v>
       </c>
       <c r="I17" s="53">
@@ -3699,7 +4183,7 @@
       <c r="J17" s="4">
         <v>18</v>
       </c>
-      <c r="K17" s="90">
+      <c r="K17" s="62">
         <v>21.2</v>
       </c>
       <c r="L17" s="53">
@@ -3728,22 +4212,22 @@
       <c r="G18" s="43">
         <v>-80</v>
       </c>
-      <c r="H18" s="93">
-        <v>0</v>
-      </c>
-      <c r="I18" s="94">
-        <v>0</v>
-      </c>
-      <c r="J18" s="95">
-        <v>0</v>
-      </c>
-      <c r="K18" s="93">
-        <v>0</v>
-      </c>
-      <c r="L18" s="94">
-        <v>0</v>
-      </c>
-      <c r="M18" s="96">
+      <c r="H18" s="64">
+        <v>0</v>
+      </c>
+      <c r="I18" s="65">
+        <v>0</v>
+      </c>
+      <c r="J18" s="66">
+        <v>0</v>
+      </c>
+      <c r="K18" s="64">
+        <v>0</v>
+      </c>
+      <c r="L18" s="65">
+        <v>0</v>
+      </c>
+      <c r="M18" s="67">
         <v>0</v>
       </c>
     </row>
@@ -3766,22 +4250,22 @@
       <c r="G19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="97">
+      <c r="H19" s="68">
         <v>8.6</v>
       </c>
-      <c r="I19" s="98">
+      <c r="I19" s="69">
         <v>5.3</v>
       </c>
-      <c r="J19" s="99">
+      <c r="J19" s="70">
         <v>-120</v>
       </c>
-      <c r="K19" s="97">
+      <c r="K19" s="68">
         <v>8.6</v>
       </c>
-      <c r="L19" s="98">
+      <c r="L19" s="69">
         <v>5.3</v>
       </c>
-      <c r="M19" s="100">
+      <c r="M19" s="71">
         <v>-120</v>
       </c>
     </row>
@@ -3809,8 +4293,8 @@
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
@@ -3819,8 +4303,8 @@
       <c r="E24" s="42"/>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>

</xml_diff>

<commit_message>
Added PWM motor control response curve
</commit_message>
<xml_diff>
--- a/Dades en Llaç obert.xlsx
+++ b/Dades en Llaç obert.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Control Automatic\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Motor  Tac. Pot. i ADC" sheetId="1" r:id="rId1"/>
     <sheet name="PWM en llaç obert" sheetId="3" r:id="rId2"/>
     <sheet name="Bodes Filtre i Derivador" sheetId="2" r:id="rId3"/>
+    <sheet name="Motor  PWM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Angle</t>
   </si>
@@ -172,12 +173,36 @@
   <si>
     <t>Escala Ton</t>
   </si>
+  <si>
+    <t>El fre distorsiona el Duty Cycle %</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>D% A</t>
+  </si>
+  <si>
+    <t>D% B</t>
+  </si>
+  <si>
+    <t>Retard A-B us</t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +277,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,8 +329,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="60">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -994,11 +1033,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,6 +1268,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1299,6 +1380,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1618,7 +1738,7 @@
   <dimension ref="A2:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F30"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3157,7 +3277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3634,79 +3754,79 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="85" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="86"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="82" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="84"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="90"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="99" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="102" t="s">
+      <c r="I3" s="106"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="100"/>
-      <c r="M3" s="103"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="109"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="95" t="s">
+      <c r="D4" s="104"/>
+      <c r="E4" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="96"/>
-      <c r="G4" s="94" t="s">
+      <c r="F4" s="102"/>
+      <c r="G4" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="104" t="s">
+      <c r="I4" s="85"/>
+      <c r="J4" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="80" t="s">
+      <c r="L4" s="85"/>
+      <c r="M4" s="86" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
-      <c r="B5" s="92"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="44" t="s">
         <v>29</v>
       </c>
@@ -3719,21 +3839,21 @@
       <c r="F5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="81"/>
+      <c r="G5" s="87"/>
       <c r="H5" s="45" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="105"/>
+      <c r="J5" s="111"/>
       <c r="K5" s="45" t="s">
         <v>29</v>
       </c>
       <c r="L5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="81"/>
+      <c r="M5" s="87"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="47">
@@ -4396,4 +4516,1057 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="13.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="114" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="118" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>-5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-5</v>
+      </c>
+      <c r="D4" s="33">
+        <f>148.3/4</f>
+        <v>37.075000000000003</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4*2*PI()</f>
+        <v>232.94909526368318</v>
+      </c>
+      <c r="F4" s="37">
+        <f>D4*60</f>
+        <v>2224.5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>246</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="120">
+        <v>100</v>
+      </c>
+      <c r="J4" s="121">
+        <v>0</v>
+      </c>
+      <c r="K4" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+    </row>
+    <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>-4.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-4.5010000000000003</v>
+      </c>
+      <c r="D5" s="34">
+        <f>122/4</f>
+        <v>30.5</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5*2*PI()</f>
+        <v>191.63715186897738</v>
+      </c>
+      <c r="F5" s="38">
+        <f>D5*60</f>
+        <v>1830</v>
+      </c>
+      <c r="G5" s="4">
+        <v>203</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4.58</v>
+      </c>
+      <c r="I5" s="34">
+        <v>93.6</v>
+      </c>
+      <c r="J5" s="4">
+        <v>6.78</v>
+      </c>
+      <c r="K5" s="79"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+    </row>
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>-4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-4.0030000000000001</v>
+      </c>
+      <c r="D6" s="35">
+        <f>102.5/4</f>
+        <v>25.625</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" ref="E6:E29" si="0">D6*2*PI()</f>
+        <v>161.00662349647689</v>
+      </c>
+      <c r="F6" s="39">
+        <f t="shared" ref="F6:F29" si="1">D6*60</f>
+        <v>1537.5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>170</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7.6</v>
+      </c>
+      <c r="I6" s="120">
+        <v>88.4</v>
+      </c>
+      <c r="J6" s="121">
+        <v>11.8</v>
+      </c>
+      <c r="K6" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="74">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="M6" s="74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>-3.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-3.5019999999999998</v>
+      </c>
+      <c r="D7" s="34">
+        <f>82/4</f>
+        <v>20.5</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>128.80529879718151</v>
+      </c>
+      <c r="F7" s="38">
+        <f t="shared" si="1"/>
+        <v>1230</v>
+      </c>
+      <c r="G7" s="4">
+        <v>138</v>
+      </c>
+      <c r="H7" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="I7" s="34">
+        <v>83.6</v>
+      </c>
+      <c r="J7" s="4">
+        <v>16.7</v>
+      </c>
+      <c r="K7" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="74">
+        <f>1000/(L6)</f>
+        <v>58.616647127784297</v>
+      </c>
+      <c r="M7" s="74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
+        <v>-3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-3.0009999999999999</v>
+      </c>
+      <c r="D8" s="35">
+        <f>64.8/4</f>
+        <v>16.2</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>101.78760197630929</v>
+      </c>
+      <c r="F8" s="39">
+        <f t="shared" si="1"/>
+        <v>972</v>
+      </c>
+      <c r="G8" s="6">
+        <v>114</v>
+      </c>
+      <c r="H8" s="5">
+        <v>12.4</v>
+      </c>
+      <c r="I8" s="120">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="J8" s="121">
+        <v>21.6</v>
+      </c>
+      <c r="K8" s="79"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>-2.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-2.5030000000000001</v>
+      </c>
+      <c r="D9" s="34">
+        <f>51.1/4</f>
+        <v>12.775</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>80.26769229921922</v>
+      </c>
+      <c r="F9" s="38">
+        <f t="shared" si="1"/>
+        <v>766.5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>87</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="I9" s="34">
+        <v>76.3</v>
+      </c>
+      <c r="J9" s="4">
+        <v>26.6</v>
+      </c>
+      <c r="K9" s="79"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+    </row>
+    <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>-2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-2</v>
+      </c>
+      <c r="D10" s="35">
+        <f>33.5/4</f>
+        <v>8.375</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>52.621676947629034</v>
+      </c>
+      <c r="F10" s="39">
+        <f t="shared" si="1"/>
+        <v>502.5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>50</v>
+      </c>
+      <c r="H10" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="I10" s="120">
+        <v>70</v>
+      </c>
+      <c r="J10" s="121">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="K10" s="79"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>-1.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-1.5029999999999999</v>
+      </c>
+      <c r="D11" s="34">
+        <f>13.75/4</f>
+        <v>3.4375</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="4">
+        <v>12</v>
+      </c>
+      <c r="H11" s="3">
+        <v>21.3</v>
+      </c>
+      <c r="I11" s="34">
+        <v>65.2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="K11" s="79"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-1.0049999999999999</v>
+      </c>
+      <c r="D12" s="35">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>24.2</v>
+      </c>
+      <c r="I12" s="120">
+        <v>60.2</v>
+      </c>
+      <c r="J12" s="121">
+        <v>42.6</v>
+      </c>
+      <c r="K12" s="79"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>-0.8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.80100000000000005</v>
+      </c>
+      <c r="D13" s="34">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>24.9</v>
+      </c>
+      <c r="I13" s="34">
+        <v>59</v>
+      </c>
+      <c r="J13" s="4">
+        <v>43.9</v>
+      </c>
+      <c r="K13" s="79"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
+        <v>-0.6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-0.60199999999999998</v>
+      </c>
+      <c r="D14" s="35">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>25.6</v>
+      </c>
+      <c r="I14" s="120">
+        <v>57.7</v>
+      </c>
+      <c r="J14" s="121">
+        <v>45.1</v>
+      </c>
+      <c r="K14" s="79"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>-0.4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-0.40300000000000002</v>
+      </c>
+      <c r="D15" s="34">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>27</v>
+      </c>
+      <c r="I15" s="34">
+        <v>55.2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>47.6</v>
+      </c>
+      <c r="K15" s="79"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="124"/>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="13">
+        <v>-0.2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>-0.20100000000000001</v>
+      </c>
+      <c r="D16" s="35">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>27.8</v>
+      </c>
+      <c r="I16" s="120">
+        <v>54</v>
+      </c>
+      <c r="J16" s="121">
+        <v>48.8</v>
+      </c>
+      <c r="K16" s="79"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-1E-3</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>29.2</v>
+      </c>
+      <c r="I17" s="34">
+        <v>51.5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>51.3</v>
+      </c>
+      <c r="K17" s="79"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D18" s="35">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>30.7</v>
+      </c>
+      <c r="I18" s="120">
+        <v>49.1</v>
+      </c>
+      <c r="J18" s="121">
+        <v>53.8</v>
+      </c>
+      <c r="K18" s="79"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="D19" s="34">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>31.4</v>
+      </c>
+      <c r="I19" s="34">
+        <v>47.8</v>
+      </c>
+      <c r="J19" s="4">
+        <v>55</v>
+      </c>
+      <c r="K19" s="79"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="35">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I20" s="120">
+        <v>45.4</v>
+      </c>
+      <c r="J20" s="121">
+        <v>57.5</v>
+      </c>
+      <c r="K20" s="79"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="D21" s="34">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>33.5</v>
+      </c>
+      <c r="I21" s="34">
+        <v>44.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>58.7</v>
+      </c>
+      <c r="K21" s="79"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D22" s="35">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>10</v>
+      </c>
+      <c r="H22" s="5">
+        <v>-21.4</v>
+      </c>
+      <c r="I22" s="120">
+        <v>38</v>
+      </c>
+      <c r="J22" s="121">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="K22" s="79"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22" s="74"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1.502</v>
+      </c>
+      <c r="D23" s="34">
+        <f>15/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
+        <v>23.561944901923447</v>
+      </c>
+      <c r="F23" s="38">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="G23" s="4">
+        <v>44</v>
+      </c>
+      <c r="H23" s="3">
+        <v>-18.600000000000001</v>
+      </c>
+      <c r="I23" s="34">
+        <v>33</v>
+      </c>
+      <c r="J23" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="K23" s="79"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="13">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="35">
+        <f>39.2/4</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>61.575216010359952</v>
+      </c>
+      <c r="F24" s="39">
+        <f t="shared" si="1"/>
+        <v>588</v>
+      </c>
+      <c r="G24" s="6">
+        <v>77</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-15.6</v>
+      </c>
+      <c r="I24" s="120">
+        <v>28</v>
+      </c>
+      <c r="J24" s="121">
+        <v>74.7</v>
+      </c>
+      <c r="K24" s="79"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="74"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="34">
+        <f>57/4</f>
+        <v>14.25</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>89.535390627309098</v>
+      </c>
+      <c r="F25" s="38">
+        <f t="shared" si="1"/>
+        <v>855</v>
+      </c>
+      <c r="G25" s="4">
+        <v>104</v>
+      </c>
+      <c r="H25" s="3">
+        <v>-13.1</v>
+      </c>
+      <c r="I25" s="34">
+        <v>23.1</v>
+      </c>
+      <c r="J25" s="4">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="K25" s="79"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="13">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3</v>
+      </c>
+      <c r="D26" s="35">
+        <f>70/4</f>
+        <v>17.5</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="F26" s="39">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
+      <c r="G26" s="6">
+        <v>120</v>
+      </c>
+      <c r="H26" s="5">
+        <v>-12.2</v>
+      </c>
+      <c r="I26" s="120">
+        <v>18.2</v>
+      </c>
+      <c r="J26" s="121">
+        <v>80.8</v>
+      </c>
+      <c r="K26" s="79"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="N26" s="74"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D27" s="34">
+        <f>85.5/4</f>
+        <v>21.375</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>134.30308594096365</v>
+      </c>
+      <c r="F27" s="38">
+        <f t="shared" si="1"/>
+        <v>1282.5</v>
+      </c>
+      <c r="G27" s="4">
+        <v>160</v>
+      </c>
+      <c r="H27" s="3">
+        <v>-8.7100000000000009</v>
+      </c>
+      <c r="I27" s="34">
+        <v>12</v>
+      </c>
+      <c r="J27" s="4">
+        <v>86.6</v>
+      </c>
+      <c r="K27" s="79"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="13">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5">
+        <v>4.0010000000000003</v>
+      </c>
+      <c r="D28" s="35">
+        <f>104.1/4</f>
+        <v>26.024999999999999</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>163.51989761934871</v>
+      </c>
+      <c r="F28" s="39">
+        <f t="shared" si="1"/>
+        <v>1561.5</v>
+      </c>
+      <c r="G28" s="6">
+        <v>193</v>
+      </c>
+      <c r="H28" s="5">
+        <v>-5.83</v>
+      </c>
+      <c r="I28" s="120">
+        <v>7.06</v>
+      </c>
+      <c r="J28" s="121">
+        <v>91.5</v>
+      </c>
+      <c r="K28" s="79"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" s="74"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4.4969999999999999</v>
+      </c>
+      <c r="D29" s="34">
+        <f>123.2/4</f>
+        <v>30.8</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="0"/>
+        <v>193.52210746113127</v>
+      </c>
+      <c r="F29" s="38">
+        <f t="shared" si="1"/>
+        <v>1848</v>
+      </c>
+      <c r="G29" s="4">
+        <v>242</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="34">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>100</v>
+      </c>
+      <c r="K29" s="79"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="14">
+        <v>5</v>
+      </c>
+      <c r="C30" s="7">
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="D30" s="36">
+        <f>148/4</f>
+        <v>37</v>
+      </c>
+      <c r="E30" s="3">
+        <f>D30*2*PI()</f>
+        <v>232.4778563656447</v>
+      </c>
+      <c r="F30" s="40">
+        <f>D30*60</f>
+        <v>2220</v>
+      </c>
+      <c r="G30" s="8">
+        <v>241</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="122">
+        <v>0</v>
+      </c>
+      <c r="J30" s="123">
+        <v>100</v>
+      </c>
+      <c r="K30" s="79"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="74"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>